<commit_message>
updated PI google scholar ID and scopus ID
</commit_message>
<xml_diff>
--- a/TPM 2023 Principal Investigators.xlsx
+++ b/TPM 2023 Principal Investigators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/jzhu986_uoa_auckland_ac_nz/Documents/Desktop/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhu/Desktop/Pub_Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{1BB81F5B-2D75-3744-9B88-696F6BB4C26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6C712A6-B52E-4F52-887D-91D8E4F5A702}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B88303E-FE54-CD4A-81E9-DBD149E50FC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="421">
   <si>
     <t>First Name</t>
   </si>
@@ -518,690 +507,836 @@
     <t>c.macinnis-ng@auckland.ac.nz</t>
   </si>
   <si>
+    <t>MacLeod</t>
+  </si>
+  <si>
+    <t>Macmillan</t>
+  </si>
+  <si>
+    <t>alex.macmillan@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Marsland</t>
+  </si>
+  <si>
+    <t>stephen.marsland@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Matheson</t>
+  </si>
+  <si>
+    <t>anna.matheson@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
+    <t>adrian.mcdonald@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Zac</t>
+  </si>
+  <si>
+    <t>McIvor</t>
+  </si>
+  <si>
+    <t>zac.mcivor@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Jeanette</t>
+  </si>
+  <si>
+    <t>McLeod</t>
+  </si>
+  <si>
+    <t>jeanette.mcleod@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>morganf@landcareresearch.co.nz</t>
+  </si>
+  <si>
+    <t>Marama</t>
+  </si>
+  <si>
+    <t>Muru-Lanning</t>
+  </si>
+  <si>
+    <t>m.murulanning@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Sereana</t>
+  </si>
+  <si>
+    <t>Naepi</t>
+  </si>
+  <si>
+    <t>s.naepi@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Nirmal</t>
+  </si>
+  <si>
+    <t>Nair</t>
+  </si>
+  <si>
+    <t>n.nair@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Dion</t>
+  </si>
+  <si>
+    <t>O’Neale</t>
+  </si>
+  <si>
+    <t>d.oneale@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>O’Sullivan</t>
+  </si>
+  <si>
+    <t>michael.osullivan@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Chrissie</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>chrissie.painting@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Parry</t>
+  </si>
+  <si>
+    <t>mparry@maths.otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Phillipps</t>
+  </si>
+  <si>
+    <t>rebecca.phillipps@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Pilkington</t>
+  </si>
+  <si>
+    <t>lisa.pilkington@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Pinkerton</t>
+  </si>
+  <si>
+    <t>Plank</t>
+  </si>
+  <si>
+    <t>michael.plank@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Postlethwaite</t>
+  </si>
+  <si>
+    <t>c.postlethwaite@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Matiu</t>
+  </si>
+  <si>
+    <t>Prebble</t>
+  </si>
+  <si>
+    <t>matiu.prebble@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Priestley</t>
+  </si>
+  <si>
+    <t>Mubashir</t>
+  </si>
+  <si>
+    <t>Qasim</t>
+  </si>
+  <si>
+    <t>Dairy NZ</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Riggs</t>
+  </si>
+  <si>
+    <t>NZ Productivity Commission</t>
+  </si>
+  <si>
+    <t>Roa</t>
+  </si>
+  <si>
+    <t>tomroa@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Roudier</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>peter.russell@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Otago University</t>
+  </si>
+  <si>
+    <t>Rhian</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>rhian.salmon@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Wellington (Kapiti Coast)</t>
+  </si>
+  <si>
+    <t>a.santure@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Sharp</t>
+  </si>
+  <si>
+    <t>el.sharp@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Dianne</t>
+  </si>
+  <si>
+    <t>Sika-Paotonu</t>
+  </si>
+  <si>
+    <t>dianne.sika-paotonu@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Inga</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>inga.smith@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Steeves</t>
+  </si>
+  <si>
+    <t>tammy.steeves@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Stewart</t>
+  </si>
+  <si>
+    <t>simon.stewart@cawthron.org.nz</t>
+  </si>
+  <si>
+    <t>Stouffer</t>
+  </si>
+  <si>
+    <t>daniel.stouffer@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Subramanian</t>
+  </si>
+  <si>
+    <t>priya.subramanian@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Talbot-Jones</t>
+  </si>
+  <si>
+    <t>julia.talbotjones@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Victoria University/ Motu affiliate</t>
+  </si>
+  <si>
+    <t>Hiran</t>
+  </si>
+  <si>
+    <t>Thabrew</t>
+  </si>
+  <si>
+    <t>h.thabrew@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Holly</t>
+  </si>
+  <si>
+    <t>Thorpe</t>
+  </si>
+  <si>
+    <t>holly.thorpe@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Tonkin</t>
+  </si>
+  <si>
+    <t>jonathan.tonkin@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Te Rerekohu</t>
+  </si>
+  <si>
+    <t>Tuterangiwhiu</t>
+  </si>
+  <si>
+    <t>wheiao.whakaaro@gmail.com</t>
+  </si>
+  <si>
+    <t>Rotorua</t>
+  </si>
+  <si>
+    <t>Rhema</t>
+  </si>
+  <si>
+    <t>Vaithianathan</t>
+  </si>
+  <si>
+    <t>rhema.vaithianathan@aut.ac.nz</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Velarde</t>
+  </si>
+  <si>
+    <t>sjvelarde@gmail.com</t>
+  </si>
+  <si>
+    <t>WSP</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Villamor</t>
+  </si>
+  <si>
+    <t>Scion</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>cameron.walker@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Leilani</t>
+  </si>
+  <si>
+    <t>leilani.walker@aut.ac.nz</t>
+  </si>
+  <si>
+    <t>Krushil</t>
+  </si>
+  <si>
+    <t>Watene</t>
+  </si>
+  <si>
+    <t>krushil.watene@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Priscilla</t>
+  </si>
+  <si>
+    <t>Wehi</t>
+  </si>
+  <si>
+    <t>priscilla.wehi@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Hēmi</t>
+  </si>
+  <si>
+    <t>Whaanga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massey University </t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Whitehead</t>
+  </si>
+  <si>
+    <t>jesse.whitehead@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>University of Waikato/Nirai Research Ltd</t>
+  </si>
+  <si>
+    <t>Ōhaupō (Waikato)</t>
+  </si>
+  <si>
+    <t>Siouxsie</t>
+  </si>
+  <si>
+    <t>Wiles</t>
+  </si>
+  <si>
+    <t>s.wiles@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phillip.wilson@canterbury.ac.nz  </t>
+  </si>
+  <si>
+    <t>Ilze</t>
+  </si>
+  <si>
+    <t>Ziedins</t>
+  </si>
+  <si>
+    <t>i.ziedins@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Uli</t>
+  </si>
+  <si>
+    <t>Zuelicke</t>
+  </si>
+  <si>
+    <t>grace.villamor@scionresearch.com</t>
+  </si>
+  <si>
+    <t>i.c.castro@massey.ac.nz</t>
+  </si>
+  <si>
+    <t>lynn.riggs@productivity.govt.nz</t>
+  </si>
+  <si>
+    <t>william.godsoe@lincoln.ac.nz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celine.cattoen-gilbert@niwa.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.t.s.hayman@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h.whaanga@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.liggins@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">matt.pinkerton@niwa.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">marcus.frean@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mubashir.qasim@dairynz.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">roudierp@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rebecca.priestley@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">binnyr@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uli.zuelicke@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">etheringtont@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j.hunter1@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">macleodc@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>possibly also Alexandra</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Hamilton/ Gisborne</t>
+  </si>
+  <si>
+    <t>Jono</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Whangarei</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Phil</t>
+  </si>
+  <si>
+    <t>Cilla</t>
+  </si>
+  <si>
+    <t>Ulrich</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Thomas?</t>
+  </si>
+  <si>
+    <t>Other versions of their first name they use</t>
+  </si>
+  <si>
+    <t>Tabi</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>andrea.tabi@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Reju</t>
+  </si>
+  <si>
+    <t>reju.sam.john@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Buarque</t>
+  </si>
+  <si>
+    <t>bbuarque@gmail.com</t>
+  </si>
+  <si>
+    <t>Kelley</t>
+  </si>
+  <si>
+    <t>dkel960@aucklanduni.ac.nz</t>
+  </si>
+  <si>
+    <t>Franca</t>
+  </si>
+  <si>
+    <t>Buelow</t>
+  </si>
+  <si>
+    <t>Virens</t>
+  </si>
+  <si>
+    <t>franca.buelow@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Beattie</t>
+  </si>
+  <si>
+    <t>alex.beattie@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Victoria University of Wellington</t>
+  </si>
+  <si>
+    <t>Aisling</t>
+  </si>
+  <si>
+    <t>Rayne</t>
+  </si>
+  <si>
+    <t>aisling.rayne@cawthron.org.nz</t>
+  </si>
+  <si>
+    <t>evelynvirens@gmail.com</t>
+  </si>
+  <si>
+    <t>Evelyn</t>
+  </si>
+  <si>
+    <t>google_scholar_id</t>
+  </si>
+  <si>
+    <t>9zBBTb0AAAAJ</t>
+  </si>
+  <si>
+    <t>TSjPmycAAAAJ</t>
+  </si>
+  <si>
+    <t>8D8W8NsAAAAJ</t>
+  </si>
+  <si>
+    <t>scopus_au_id</t>
+  </si>
+  <si>
+    <t>Ic0ntsUAAAAJ</t>
+  </si>
+  <si>
+    <t>Xt1AACMAAAAJ</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>N2b7dCcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Santure</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1jc3_IAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHwGXBwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>Catriona</t>
-  </si>
-  <si>
-    <t>MacLeod</t>
-  </si>
-  <si>
-    <t>Macmillan</t>
-  </si>
-  <si>
-    <t>alex.macmillan@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Stephen</t>
-  </si>
-  <si>
-    <t>Marsland</t>
-  </si>
-  <si>
-    <t>stephen.marsland@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Matheson</t>
-  </si>
-  <si>
-    <t>anna.matheson@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Adrian</t>
-  </si>
-  <si>
-    <t>McDonald</t>
-  </si>
-  <si>
-    <t>adrian.mcdonald@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Zac</t>
-  </si>
-  <si>
-    <t>McIvor</t>
-  </si>
-  <si>
-    <t>zac.mcivor@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Jeanette</t>
-  </si>
-  <si>
-    <t>McLeod</t>
-  </si>
-  <si>
-    <t>jeanette.mcleod@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Fraser</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>morganf@landcareresearch.co.nz</t>
-  </si>
-  <si>
-    <t>Marama</t>
-  </si>
-  <si>
-    <t>Muru-Lanning</t>
-  </si>
-  <si>
-    <t>m.murulanning@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Sereana</t>
-  </si>
-  <si>
-    <t>Naepi</t>
-  </si>
-  <si>
-    <t>s.naepi@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Nirmal</t>
-  </si>
-  <si>
-    <t>Nair</t>
-  </si>
-  <si>
-    <t>n.nair@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Dion</t>
-  </si>
-  <si>
-    <t>O’Neale</t>
-  </si>
-  <si>
-    <t>d.oneale@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>O’Sullivan</t>
-  </si>
-  <si>
-    <t>michael.osullivan@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Chrissie</t>
-  </si>
-  <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>chrissie.painting@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Parry</t>
-  </si>
-  <si>
-    <t>mparry@maths.otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Rebecca</t>
-  </si>
-  <si>
-    <t>Phillipps</t>
-  </si>
-  <si>
-    <t>rebecca.phillipps@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>Pilkington</t>
-  </si>
-  <si>
-    <t>lisa.pilkington@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Pinkerton</t>
-  </si>
-  <si>
-    <t>Plank</t>
-  </si>
-  <si>
-    <t>michael.plank@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Claire</t>
-  </si>
-  <si>
-    <t>Postlethwaite</t>
-  </si>
-  <si>
-    <t>c.postlethwaite@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Matiu</t>
-  </si>
-  <si>
-    <t>Prebble</t>
-  </si>
-  <si>
-    <t>matiu.prebble@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Priestley</t>
-  </si>
-  <si>
-    <t>Mubashir</t>
-  </si>
-  <si>
-    <t>Qasim</t>
-  </si>
-  <si>
-    <t>Dairy NZ</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Riggs</t>
-  </si>
-  <si>
-    <t>NZ Productivity Commission</t>
-  </si>
-  <si>
-    <t>Roa</t>
-  </si>
-  <si>
-    <t>tomroa@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>Roudier</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Russell</t>
-  </si>
-  <si>
-    <t>peter.russell@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Otago University</t>
-  </si>
-  <si>
-    <t>Rhian</t>
-  </si>
-  <si>
-    <t>Salmon</t>
-  </si>
-  <si>
-    <t>rhian.salmon@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Wellington (Kapiti Coast)</t>
-  </si>
-  <si>
-    <t>Santure</t>
-  </si>
-  <si>
-    <t>a.santure@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Sharp</t>
-  </si>
-  <si>
-    <t>el.sharp@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Dianne</t>
-  </si>
-  <si>
-    <t>Sika-Paotonu</t>
-  </si>
-  <si>
-    <t>dianne.sika-paotonu@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Inga</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>inga.smith@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Tammy</t>
-  </si>
-  <si>
-    <t>Steeves</t>
-  </si>
-  <si>
-    <t>tammy.steeves@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Stewart</t>
-  </si>
-  <si>
-    <t>simon.stewart@cawthron.org.nz</t>
-  </si>
-  <si>
-    <t>Stouffer</t>
-  </si>
-  <si>
-    <t>daniel.stouffer@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Priya</t>
-  </si>
-  <si>
-    <t>Subramanian</t>
-  </si>
-  <si>
-    <t>priya.subramanian@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Talbot-Jones</t>
-  </si>
-  <si>
-    <t>julia.talbotjones@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Victoria University/ Motu affiliate</t>
-  </si>
-  <si>
-    <t>Hiran</t>
-  </si>
-  <si>
-    <t>Thabrew</t>
-  </si>
-  <si>
-    <t>h.thabrew@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Holly</t>
-  </si>
-  <si>
-    <t>Thorpe</t>
-  </si>
-  <si>
-    <t>holly.thorpe@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Tonkin</t>
-  </si>
-  <si>
-    <t>jonathan.tonkin@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Te Rerekohu</t>
-  </si>
-  <si>
-    <t>Tuterangiwhiu</t>
-  </si>
-  <si>
-    <t>wheiao.whakaaro@gmail.com</t>
-  </si>
-  <si>
-    <t>Rotorua</t>
-  </si>
-  <si>
-    <t>Rhema</t>
-  </si>
-  <si>
-    <t>Vaithianathan</t>
-  </si>
-  <si>
-    <t>rhema.vaithianathan@aut.ac.nz</t>
-  </si>
-  <si>
-    <t>Sandra</t>
-  </si>
-  <si>
-    <t>Velarde</t>
-  </si>
-  <si>
-    <t>sjvelarde@gmail.com</t>
-  </si>
-  <si>
-    <t>WSP</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>Villamor</t>
-  </si>
-  <si>
-    <t>Scion</t>
-  </si>
-  <si>
-    <t>Cameron</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
-    <t>cameron.walker@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Leilani</t>
-  </si>
-  <si>
-    <t>leilani.walker@aut.ac.nz</t>
-  </si>
-  <si>
-    <t>Krushil</t>
-  </si>
-  <si>
-    <t>Watene</t>
-  </si>
-  <si>
-    <t>krushil.watene@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Priscilla</t>
-  </si>
-  <si>
-    <t>Wehi</t>
-  </si>
-  <si>
-    <t>priscilla.wehi@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Hēmi</t>
-  </si>
-  <si>
-    <t>Whaanga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Massey University </t>
-  </si>
-  <si>
-    <t>Jesse</t>
-  </si>
-  <si>
-    <t>Whitehead</t>
-  </si>
-  <si>
-    <t>jesse.whitehead@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>University of Waikato/Nirai Research Ltd</t>
-  </si>
-  <si>
-    <t>Ōhaupō (Waikato)</t>
-  </si>
-  <si>
-    <t>Siouxsie</t>
-  </si>
-  <si>
-    <t>Wiles</t>
-  </si>
-  <si>
-    <t>s.wiles@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Phillip</t>
-  </si>
-  <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phillip.wilson@canterbury.ac.nz  </t>
-  </si>
-  <si>
-    <t>Ilze</t>
-  </si>
-  <si>
-    <t>Ziedins</t>
-  </si>
-  <si>
-    <t>i.ziedins@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Uli</t>
-  </si>
-  <si>
-    <t>Zuelicke</t>
-  </si>
-  <si>
-    <t>grace.villamor@scionresearch.com</t>
-  </si>
-  <si>
-    <t>i.c.castro@massey.ac.nz</t>
-  </si>
-  <si>
-    <t>lynn.riggs@productivity.govt.nz</t>
-  </si>
-  <si>
-    <t>william.godsoe@lincoln.ac.nz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">celine.cattoen-gilbert@niwa.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d.t.s.hayman@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">h.whaanga@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.liggins@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">matt.pinkerton@niwa.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">marcus.frean@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mubashir.qasim@dairynz.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">roudierp@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rebecca.priestley@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">binnyr@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uli.zuelicke@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">etheringtont@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">j.hunter1@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">macleodc@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t>Christina</t>
-  </si>
-  <si>
-    <t>possibly also Alexandra</t>
-  </si>
-  <si>
-    <t>Cam</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Hamilton/ Gisborne</t>
-  </si>
-  <si>
-    <t>Jono</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Whangarei</t>
-  </si>
-  <si>
-    <t>Nicholas</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Phil</t>
-  </si>
-  <si>
-    <t>Cilla</t>
-  </si>
-  <si>
-    <t>Ulrich</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Thomas?</t>
-  </si>
-  <si>
-    <t>Other versions of their first name they use</t>
-  </si>
-  <si>
-    <t>Tabi</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>andrea.tabi@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Reju</t>
-  </si>
-  <si>
-    <t>reju.sam.john@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Bernardo</t>
-  </si>
-  <si>
-    <t>Buarque</t>
-  </si>
-  <si>
-    <t>bbuarque@gmail.com</t>
-  </si>
-  <si>
-    <t>Kelley</t>
-  </si>
-  <si>
-    <t>dkel960@aucklanduni.ac.nz</t>
-  </si>
-  <si>
-    <t>Franca</t>
-  </si>
-  <si>
-    <t>Buelow</t>
-  </si>
-  <si>
-    <t>Virens</t>
-  </si>
-  <si>
-    <t>franca.buelow@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Beattie</t>
-  </si>
-  <si>
-    <t>alex.beattie@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Victoria University of Wellington</t>
-  </si>
-  <si>
-    <t>Aisling</t>
-  </si>
-  <si>
-    <t>Rayne</t>
-  </si>
-  <si>
-    <t>aisling.rayne@cawthron.org.nz</t>
-  </si>
-  <si>
-    <t>evelynvirens@gmail.com</t>
-  </si>
-  <si>
-    <t>Evelyn</t>
-  </si>
-  <si>
-    <t>google_scholar_id</t>
-  </si>
-  <si>
-    <t>9zBBTb0AAAAJ</t>
-  </si>
-  <si>
-    <t>TSjPmycAAAAJ</t>
-  </si>
-  <si>
-    <t>8D8W8NsAAAAJ</t>
-  </si>
-  <si>
-    <t>scopus_au_id</t>
-  </si>
-  <si>
-    <t>Ic0ntsUAAAAJ</t>
-  </si>
-  <si>
-    <t>Xt1AACMAAAAJ</t>
-  </si>
-  <si>
-    <t>skip</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFsg92IAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K9stBsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ymcd_j8AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>U075c-cAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>3svcBDsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1RfyVk4AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>q9BV9soAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HfQdgrcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>pqW61O0AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaderGYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>3SsqlCkAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0FInvU4AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>XCK_D0oAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>sE2Je-oAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VhX3VbwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>JhDH40UAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>mJlK_dwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PkUDCPsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZiUSYlMAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>g8DH5gYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>yINTHKsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>jKnJDPMAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVEIwcQAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>pHjNU0gAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>hBdEqeYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mtn0TIwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>80v_y-YAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>lqL9DsoAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>KuDLalcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ze-7kTYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>eLYlC84AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>qRwdoDkAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>yi87D2cAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1210,14 +1345,14 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1225,7 +1360,7 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1239,14 +1374,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1256,13 +1391,26 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1278,7 +1426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1295,10 +1443,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1318,7 +1472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1616,21 +1770,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8B157A-D10D-D949-B41A-E7AC1C9C79E8}">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="20.625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
-    <col min="5" max="5" width="34.625" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1638,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1653,28 +1807,28 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>53</v>
@@ -1684,7 +1838,7 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I2">
         <v>56250119900</v>
@@ -1712,7 +1866,7 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I3">
         <v>55545943200</v>
@@ -1727,10 +1881,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -1739,10 +1893,10 @@
         <v>23</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I4">
         <v>7005704384</v>
@@ -1770,7 +1924,7 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I5">
         <v>18233378900</v>
@@ -1811,10 +1965,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
@@ -1824,7 +1978,7 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I7">
         <v>7005851367</v>
@@ -1839,10 +1993,10 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>236</v>
+        <v>384</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>49</v>
@@ -1851,21 +2005,26 @@
         <v>9</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="I8">
+        <v>14219508100</v>
+      </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
@@ -1874,11 +2033,16 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>333</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="I9">
+        <v>7402887425</v>
+      </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1898,21 +2062,26 @@
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="I10">
+        <v>6603293321</v>
+      </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>160</v>
+        <v>387</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>41</v>
@@ -1920,9 +2089,14 @@
       <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="I11">
+        <v>8688520200</v>
+      </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1934,7 +2108,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>62</v>
@@ -1942,21 +2116,26 @@
       <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="I12">
+        <v>9632564900</v>
+      </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>132</v>
@@ -1965,23 +2144,28 @@
         <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>195</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I13">
+        <v>56030897200</v>
+      </c>
       <c r="J13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -1989,9 +2173,14 @@
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="I14">
+        <v>8590273100</v>
+      </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2012,11 +2201,16 @@
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>334</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="I15">
+        <v>16241337300</v>
+      </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2025,10 +2219,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>53</v>
@@ -2036,9 +2230,14 @@
       <c r="F16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="I16">
+        <v>8395488800</v>
+      </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2058,9 +2257,14 @@
       <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="I17">
+        <v>36668233300</v>
+      </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2081,8 +2285,11 @@
         <v>9</v>
       </c>
       <c r="H18" s="3"/>
+      <c r="I18">
+        <v>57287842200</v>
+      </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2094,7 +2301,7 @@
         <v>114</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -2103,23 +2310,28 @@
         <v>59</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="H19" s="4"/>
+        <v>335</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="I19">
+        <v>24376017100</v>
+      </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>22</v>
@@ -2127,21 +2339,26 @@
       <c r="F20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I20">
+        <v>14322266400</v>
+      </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>18</v>
@@ -2149,9 +2366,14 @@
       <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="I21">
+        <v>57391641100</v>
+      </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2171,9 +2393,14 @@
       <c r="F22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="I22">
+        <v>23988357400</v>
+      </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2193,21 +2420,26 @@
       <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="I23">
+        <v>36704525400</v>
+      </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
@@ -2215,21 +2447,26 @@
       <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I24">
+        <v>56602470900</v>
+      </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>41</v>
@@ -2238,9 +2475,14 @@
         <v>9</v>
       </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="I25">
+        <v>55114316000</v>
+      </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2261,9 +2503,14 @@
         <v>59</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="I26">
+        <v>7004092131</v>
+      </c>
       <c r="J26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2284,9 +2531,14 @@
         <v>28</v>
       </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="I27">
+        <v>7004267866</v>
+      </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2307,32 +2559,42 @@
         <v>42</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="I28">
+        <v>56928257900</v>
+      </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="I29">
+        <v>14629692200</v>
+      </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2353,9 +2615,14 @@
         <v>9</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I30">
+        <v>8902993900</v>
+      </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2377,43 +2644,49 @@
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="3"/>
+      <c r="I31">
+        <v>58313215900</v>
+      </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="3"/>
+      <c r="I32">
+        <v>35365484000</v>
+      </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -2421,9 +2694,14 @@
       <c r="F33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="I33">
+        <v>17339743000</v>
+      </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2444,44 +2722,54 @@
         <v>23</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="I34">
+        <v>57203528456</v>
+      </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="I35">
+        <v>12143371300</v>
+      </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>18</v>
@@ -2491,20 +2779,23 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="4"/>
+      <c r="I36">
+        <v>6603639295</v>
+      </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>22</v>
@@ -2514,43 +2805,51 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="4"/>
+      <c r="I37">
+        <v>25925460000</v>
+      </c>
       <c r="J37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="13" customFormat="1">
+      <c r="A38" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="4"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="I38" s="13">
+        <v>7102400791</v>
+      </c>
       <c r="J38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>53</v>
@@ -2560,30 +2859,38 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="3"/>
+      <c r="I39">
+        <v>14120027100</v>
+      </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="I40">
+        <v>57204169345</v>
+      </c>
       <c r="J40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2605,8 +2912,11 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="4"/>
+      <c r="I41">
+        <v>57270034900</v>
+      </c>
       <c r="J41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2618,7 +2928,7 @@
         <v>134</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
@@ -2627,21 +2937,26 @@
         <v>9</v>
       </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I42">
+        <v>56461966900</v>
+      </c>
       <c r="J42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>53</v>
@@ -2650,34 +2965,44 @@
         <v>42</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="H43" s="4"/>
+        <v>337</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="I43">
+        <v>35575180300</v>
+      </c>
       <c r="J43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="8"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I44">
+        <v>57201465027</v>
+      </c>
       <c r="J44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2699,8 +3024,11 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="3"/>
+      <c r="I45">
+        <v>57216492145</v>
+      </c>
       <c r="J45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2721,9 +3049,14 @@
         <v>9</v>
       </c>
       <c r="G46" s="8"/>
-      <c r="H46" s="3"/>
+      <c r="H46" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="I46">
+        <v>36617114700</v>
+      </c>
       <c r="J46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2744,21 +3077,26 @@
         <v>9</v>
       </c>
       <c r="G47" s="8"/>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="I47">
+        <v>55877647600</v>
+      </c>
       <c r="J47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>49</v>
@@ -2768,8 +3106,11 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="4"/>
+      <c r="I48">
+        <v>55612294300</v>
+      </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2790,21 +3131,26 @@
         <v>28</v>
       </c>
       <c r="G49" s="8"/>
-      <c r="H49" s="3"/>
+      <c r="H49" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I49">
+        <v>57193958261</v>
+      </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>141</v>
@@ -2813,9 +3159,14 @@
         <v>9</v>
       </c>
       <c r="G50" s="8"/>
-      <c r="H50" s="3"/>
+      <c r="H50" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="I50">
+        <v>57190274432</v>
+      </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2827,7 +3178,7 @@
         <v>146</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>147</v>
@@ -2836,21 +3187,26 @@
         <v>9</v>
       </c>
       <c r="G51" s="8"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="I51">
+        <v>24474607700</v>
+      </c>
       <c r="J51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
@@ -2859,32 +3215,40 @@
         <v>9</v>
       </c>
       <c r="G52" s="8"/>
-      <c r="H52" s="3"/>
+      <c r="H52" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="I52">
+        <v>55441246800</v>
+      </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="4"/>
+      <c r="I53">
+        <v>57225742769</v>
+      </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2912,14 +3276,14 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>18</v>
@@ -2942,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>27</v>
@@ -3003,14 +3367,14 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>53</v>
@@ -3026,14 +3390,14 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>22</v>
@@ -3042,7 +3406,7 @@
         <v>23</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H60" s="4"/>
       <c r="J60">
@@ -3051,14 +3415,14 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>62</v>
@@ -3143,14 +3507,14 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>18</v>
@@ -3159,7 +3523,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H65" s="4"/>
       <c r="J65">
@@ -3168,14 +3532,14 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>53</v>
@@ -3184,26 +3548,26 @@
         <v>42</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H66" s="4"/>
       <c r="J66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" ht="17">
       <c r="A67" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>14</v>
@@ -3229,7 +3593,7 @@
         <v>70</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G68" s="8"/>
       <c r="H68" s="4"/>
@@ -3239,7 +3603,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
@@ -3264,14 +3628,14 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>18</v>
@@ -3333,23 +3697,23 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H73" s="4"/>
       <c r="J73">
@@ -3358,14 +3722,14 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>53</v>
@@ -3374,7 +3738,7 @@
         <v>42</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H74" s="3"/>
       <c r="J74">
@@ -3383,14 +3747,14 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>41</v>
@@ -3406,14 +3770,14 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>22</v>
@@ -3422,7 +3786,7 @@
         <v>23</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H76" s="4"/>
       <c r="J76">
@@ -3431,14 +3795,14 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>49</v>
@@ -3507,7 +3871,7 @@
         <v>40</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>41</v>
@@ -3523,14 +3887,14 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>18</v>
@@ -3546,14 +3910,14 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>27</v>
@@ -3569,14 +3933,14 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>141</v>
@@ -3592,20 +3956,20 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G84" s="8"/>
       <c r="H84" s="4"/>
@@ -3638,20 +4002,20 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="F86" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G86" s="8"/>
       <c r="H86" s="4"/>
@@ -3661,14 +4025,14 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>49</v>
@@ -3707,14 +4071,14 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>128</v>
@@ -3730,14 +4094,14 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>18</v>
@@ -3776,14 +4140,14 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>27</v>
@@ -3799,14 +4163,14 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>53</v>
@@ -3822,20 +4186,20 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="4"/>
@@ -3875,7 +4239,7 @@
         <v>82</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>41</v>
@@ -3884,7 +4248,7 @@
         <v>42</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H96" s="4"/>
       <c r="J96">
@@ -3897,10 +4261,10 @@
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>132</v>
@@ -3941,14 +4305,14 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>27</v>
@@ -3957,7 +4321,7 @@
         <v>28</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H99" s="3"/>
       <c r="J99">
@@ -3973,7 +4337,7 @@
         <v>95</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>96</v>
@@ -3982,7 +4346,7 @@
         <v>42</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H100" s="4"/>
       <c r="J100">
@@ -3991,14 +4355,14 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>22</v>
@@ -4007,7 +4371,7 @@
         <v>23</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H101" s="3"/>
       <c r="J101">
@@ -4016,14 +4380,14 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>53</v>
@@ -4036,16 +4400,16 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B103" t="s">
+        <v>355</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>359</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>18</v>
@@ -4056,13 +4420,13 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>362</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>38</v>
@@ -4076,10 +4440,10 @@
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>18</v>
@@ -4090,16 +4454,16 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J106">
         <v>1</v>
@@ -4107,13 +4471,13 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D107" s="4" t="s">
         <v>366</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>53</v>
@@ -4127,13 +4491,13 @@
         <v>135</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -4141,13 +4505,13 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>372</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>128</v>
@@ -4157,9 +4521,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F102">
+  <sortState ref="A2:F102">
     <sortCondition ref="A2:A102"/>
   </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
update on google scholar result fill
</commit_message>
<xml_diff>
--- a/TPM 2023 Principal Investigators.xlsx
+++ b/TPM 2023 Principal Investigators.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/jzhu986_uoa_auckland_ac_nz/Documents/Desktop/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzhu986\PycharmProjects\Pub_Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{1BB81F5B-2D75-3744-9B88-696F6BB4C26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6C712A6-B52E-4F52-887D-91D8E4F5A702}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A7CA94-E630-4AA2-93DC-41098718EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="421">
   <si>
     <t>First Name</t>
   </si>
@@ -518,686 +507,831 @@
     <t>c.macinnis-ng@auckland.ac.nz</t>
   </si>
   <si>
+    <t>MacLeod</t>
+  </si>
+  <si>
+    <t>Macmillan</t>
+  </si>
+  <si>
+    <t>alex.macmillan@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Marsland</t>
+  </si>
+  <si>
+    <t>stephen.marsland@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Matheson</t>
+  </si>
+  <si>
+    <t>anna.matheson@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
+    <t>adrian.mcdonald@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Zac</t>
+  </si>
+  <si>
+    <t>McIvor</t>
+  </si>
+  <si>
+    <t>zac.mcivor@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Jeanette</t>
+  </si>
+  <si>
+    <t>McLeod</t>
+  </si>
+  <si>
+    <t>jeanette.mcleod@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>morganf@landcareresearch.co.nz</t>
+  </si>
+  <si>
+    <t>Marama</t>
+  </si>
+  <si>
+    <t>Muru-Lanning</t>
+  </si>
+  <si>
+    <t>m.murulanning@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Sereana</t>
+  </si>
+  <si>
+    <t>Naepi</t>
+  </si>
+  <si>
+    <t>s.naepi@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Nirmal</t>
+  </si>
+  <si>
+    <t>Nair</t>
+  </si>
+  <si>
+    <t>n.nair@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Dion</t>
+  </si>
+  <si>
+    <t>O’Neale</t>
+  </si>
+  <si>
+    <t>d.oneale@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>O’Sullivan</t>
+  </si>
+  <si>
+    <t>michael.osullivan@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Chrissie</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>chrissie.painting@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Parry</t>
+  </si>
+  <si>
+    <t>mparry@maths.otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Phillipps</t>
+  </si>
+  <si>
+    <t>rebecca.phillipps@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Pilkington</t>
+  </si>
+  <si>
+    <t>lisa.pilkington@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Pinkerton</t>
+  </si>
+  <si>
+    <t>Plank</t>
+  </si>
+  <si>
+    <t>michael.plank@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Postlethwaite</t>
+  </si>
+  <si>
+    <t>c.postlethwaite@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Matiu</t>
+  </si>
+  <si>
+    <t>Prebble</t>
+  </si>
+  <si>
+    <t>matiu.prebble@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Priestley</t>
+  </si>
+  <si>
+    <t>Mubashir</t>
+  </si>
+  <si>
+    <t>Qasim</t>
+  </si>
+  <si>
+    <t>Dairy NZ</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Riggs</t>
+  </si>
+  <si>
+    <t>NZ Productivity Commission</t>
+  </si>
+  <si>
+    <t>Roa</t>
+  </si>
+  <si>
+    <t>tomroa@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Roudier</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>peter.russell@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Otago University</t>
+  </si>
+  <si>
+    <t>Rhian</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>rhian.salmon@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Wellington (Kapiti Coast)</t>
+  </si>
+  <si>
+    <t>a.santure@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Sharp</t>
+  </si>
+  <si>
+    <t>el.sharp@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Dianne</t>
+  </si>
+  <si>
+    <t>Sika-Paotonu</t>
+  </si>
+  <si>
+    <t>dianne.sika-paotonu@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Inga</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>inga.smith@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Steeves</t>
+  </si>
+  <si>
+    <t>tammy.steeves@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Stewart</t>
+  </si>
+  <si>
+    <t>simon.stewart@cawthron.org.nz</t>
+  </si>
+  <si>
+    <t>Stouffer</t>
+  </si>
+  <si>
+    <t>daniel.stouffer@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Subramanian</t>
+  </si>
+  <si>
+    <t>priya.subramanian@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Talbot-Jones</t>
+  </si>
+  <si>
+    <t>julia.talbotjones@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Victoria University/ Motu affiliate</t>
+  </si>
+  <si>
+    <t>Hiran</t>
+  </si>
+  <si>
+    <t>Thabrew</t>
+  </si>
+  <si>
+    <t>h.thabrew@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Holly</t>
+  </si>
+  <si>
+    <t>Thorpe</t>
+  </si>
+  <si>
+    <t>holly.thorpe@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Tonkin</t>
+  </si>
+  <si>
+    <t>jonathan.tonkin@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Te Rerekohu</t>
+  </si>
+  <si>
+    <t>Tuterangiwhiu</t>
+  </si>
+  <si>
+    <t>wheiao.whakaaro@gmail.com</t>
+  </si>
+  <si>
+    <t>Rotorua</t>
+  </si>
+  <si>
+    <t>Rhema</t>
+  </si>
+  <si>
+    <t>Vaithianathan</t>
+  </si>
+  <si>
+    <t>rhema.vaithianathan@aut.ac.nz</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Velarde</t>
+  </si>
+  <si>
+    <t>sjvelarde@gmail.com</t>
+  </si>
+  <si>
+    <t>WSP</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Villamor</t>
+  </si>
+  <si>
+    <t>Scion</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>cameron.walker@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Leilani</t>
+  </si>
+  <si>
+    <t>leilani.walker@aut.ac.nz</t>
+  </si>
+  <si>
+    <t>Krushil</t>
+  </si>
+  <si>
+    <t>Watene</t>
+  </si>
+  <si>
+    <t>krushil.watene@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Priscilla</t>
+  </si>
+  <si>
+    <t>Wehi</t>
+  </si>
+  <si>
+    <t>priscilla.wehi@otago.ac.nz</t>
+  </si>
+  <si>
+    <t>Hēmi</t>
+  </si>
+  <si>
+    <t>Whaanga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massey University </t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Whitehead</t>
+  </si>
+  <si>
+    <t>jesse.whitehead@waikato.ac.nz</t>
+  </si>
+  <si>
+    <t>University of Waikato/Nirai Research Ltd</t>
+  </si>
+  <si>
+    <t>Ōhaupō (Waikato)</t>
+  </si>
+  <si>
+    <t>Siouxsie</t>
+  </si>
+  <si>
+    <t>Wiles</t>
+  </si>
+  <si>
+    <t>s.wiles@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phillip.wilson@canterbury.ac.nz  </t>
+  </si>
+  <si>
+    <t>Ilze</t>
+  </si>
+  <si>
+    <t>Ziedins</t>
+  </si>
+  <si>
+    <t>i.ziedins@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Uli</t>
+  </si>
+  <si>
+    <t>Zuelicke</t>
+  </si>
+  <si>
+    <t>grace.villamor@scionresearch.com</t>
+  </si>
+  <si>
+    <t>i.c.castro@massey.ac.nz</t>
+  </si>
+  <si>
+    <t>lynn.riggs@productivity.govt.nz</t>
+  </si>
+  <si>
+    <t>william.godsoe@lincoln.ac.nz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celine.cattoen-gilbert@niwa.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.t.s.hayman@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h.whaanga@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.liggins@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">matt.pinkerton@niwa.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">marcus.frean@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mubashir.qasim@dairynz.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">roudierp@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rebecca.priestley@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">binnyr@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uli.zuelicke@vuw.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">etheringtont@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j.hunter1@massey.ac.nz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">macleodc@landcareresearch.co.nz </t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>possibly also Alexandra</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Hamilton/ Gisborne</t>
+  </si>
+  <si>
+    <t>Jono</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Whangarei</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Phil</t>
+  </si>
+  <si>
+    <t>Cilla</t>
+  </si>
+  <si>
+    <t>Ulrich</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Thomas?</t>
+  </si>
+  <si>
+    <t>Other versions of their first name they use</t>
+  </si>
+  <si>
+    <t>Tabi</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>andrea.tabi@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Reju</t>
+  </si>
+  <si>
+    <t>reju.sam.john@auckland.ac.nz</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Buarque</t>
+  </si>
+  <si>
+    <t>bbuarque@gmail.com</t>
+  </si>
+  <si>
+    <t>Kelley</t>
+  </si>
+  <si>
+    <t>dkel960@aucklanduni.ac.nz</t>
+  </si>
+  <si>
+    <t>Franca</t>
+  </si>
+  <si>
+    <t>Buelow</t>
+  </si>
+  <si>
+    <t>Virens</t>
+  </si>
+  <si>
+    <t>franca.buelow@canterbury.ac.nz</t>
+  </si>
+  <si>
+    <t>Beattie</t>
+  </si>
+  <si>
+    <t>alex.beattie@vuw.ac.nz</t>
+  </si>
+  <si>
+    <t>Victoria University of Wellington</t>
+  </si>
+  <si>
+    <t>Aisling</t>
+  </si>
+  <si>
+    <t>Rayne</t>
+  </si>
+  <si>
+    <t>aisling.rayne@cawthron.org.nz</t>
+  </si>
+  <si>
+    <t>evelynvirens@gmail.com</t>
+  </si>
+  <si>
+    <t>Evelyn</t>
+  </si>
+  <si>
+    <t>google_scholar_id</t>
+  </si>
+  <si>
+    <t>9zBBTb0AAAAJ</t>
+  </si>
+  <si>
+    <t>TSjPmycAAAAJ</t>
+  </si>
+  <si>
+    <t>8D8W8NsAAAAJ</t>
+  </si>
+  <si>
+    <t>scopus_au_id</t>
+  </si>
+  <si>
+    <t>Ic0ntsUAAAAJ</t>
+  </si>
+  <si>
+    <t>Xt1AACMAAAAJ</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>N2b7dCcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Santure</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1jc3_IAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZHwGXBwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>Catriona</t>
-  </si>
-  <si>
-    <t>MacLeod</t>
-  </si>
-  <si>
-    <t>Macmillan</t>
-  </si>
-  <si>
-    <t>alex.macmillan@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Stephen</t>
-  </si>
-  <si>
-    <t>Marsland</t>
-  </si>
-  <si>
-    <t>stephen.marsland@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Matheson</t>
-  </si>
-  <si>
-    <t>anna.matheson@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Adrian</t>
-  </si>
-  <si>
-    <t>McDonald</t>
-  </si>
-  <si>
-    <t>adrian.mcdonald@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Zac</t>
-  </si>
-  <si>
-    <t>McIvor</t>
-  </si>
-  <si>
-    <t>zac.mcivor@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Jeanette</t>
-  </si>
-  <si>
-    <t>McLeod</t>
-  </si>
-  <si>
-    <t>jeanette.mcleod@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Fraser</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>morganf@landcareresearch.co.nz</t>
-  </si>
-  <si>
-    <t>Marama</t>
-  </si>
-  <si>
-    <t>Muru-Lanning</t>
-  </si>
-  <si>
-    <t>m.murulanning@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Sereana</t>
-  </si>
-  <si>
-    <t>Naepi</t>
-  </si>
-  <si>
-    <t>s.naepi@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Nirmal</t>
-  </si>
-  <si>
-    <t>Nair</t>
-  </si>
-  <si>
-    <t>n.nair@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Dion</t>
-  </si>
-  <si>
-    <t>O’Neale</t>
-  </si>
-  <si>
-    <t>d.oneale@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>O’Sullivan</t>
-  </si>
-  <si>
-    <t>michael.osullivan@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Chrissie</t>
-  </si>
-  <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>chrissie.painting@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Parry</t>
-  </si>
-  <si>
-    <t>mparry@maths.otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Rebecca</t>
-  </si>
-  <si>
-    <t>Phillipps</t>
-  </si>
-  <si>
-    <t>rebecca.phillipps@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>Pilkington</t>
-  </si>
-  <si>
-    <t>lisa.pilkington@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Pinkerton</t>
-  </si>
-  <si>
-    <t>Plank</t>
-  </si>
-  <si>
-    <t>michael.plank@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Claire</t>
-  </si>
-  <si>
-    <t>Postlethwaite</t>
-  </si>
-  <si>
-    <t>c.postlethwaite@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Matiu</t>
-  </si>
-  <si>
-    <t>Prebble</t>
-  </si>
-  <si>
-    <t>matiu.prebble@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Priestley</t>
-  </si>
-  <si>
-    <t>Mubashir</t>
-  </si>
-  <si>
-    <t>Qasim</t>
-  </si>
-  <si>
-    <t>Dairy NZ</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Riggs</t>
-  </si>
-  <si>
-    <t>NZ Productivity Commission</t>
-  </si>
-  <si>
-    <t>Roa</t>
-  </si>
-  <si>
-    <t>tomroa@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>Roudier</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
-    <t>Russell</t>
-  </si>
-  <si>
-    <t>peter.russell@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Otago University</t>
-  </si>
-  <si>
-    <t>Rhian</t>
-  </si>
-  <si>
-    <t>Salmon</t>
-  </si>
-  <si>
-    <t>rhian.salmon@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Wellington (Kapiti Coast)</t>
-  </si>
-  <si>
-    <t>Santure</t>
-  </si>
-  <si>
-    <t>a.santure@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Sharp</t>
-  </si>
-  <si>
-    <t>el.sharp@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Dianne</t>
-  </si>
-  <si>
-    <t>Sika-Paotonu</t>
-  </si>
-  <si>
-    <t>dianne.sika-paotonu@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Inga</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>inga.smith@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Tammy</t>
-  </si>
-  <si>
-    <t>Steeves</t>
-  </si>
-  <si>
-    <t>tammy.steeves@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Stewart</t>
-  </si>
-  <si>
-    <t>simon.stewart@cawthron.org.nz</t>
-  </si>
-  <si>
-    <t>Stouffer</t>
-  </si>
-  <si>
-    <t>daniel.stouffer@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Priya</t>
-  </si>
-  <si>
-    <t>Subramanian</t>
-  </si>
-  <si>
-    <t>priya.subramanian@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Talbot-Jones</t>
-  </si>
-  <si>
-    <t>julia.talbotjones@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Victoria University/ Motu affiliate</t>
-  </si>
-  <si>
-    <t>Hiran</t>
-  </si>
-  <si>
-    <t>Thabrew</t>
-  </si>
-  <si>
-    <t>h.thabrew@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Holly</t>
-  </si>
-  <si>
-    <t>Thorpe</t>
-  </si>
-  <si>
-    <t>holly.thorpe@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Tonkin</t>
-  </si>
-  <si>
-    <t>jonathan.tonkin@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Te Rerekohu</t>
-  </si>
-  <si>
-    <t>Tuterangiwhiu</t>
-  </si>
-  <si>
-    <t>wheiao.whakaaro@gmail.com</t>
-  </si>
-  <si>
-    <t>Rotorua</t>
-  </si>
-  <si>
-    <t>Rhema</t>
-  </si>
-  <si>
-    <t>Vaithianathan</t>
-  </si>
-  <si>
-    <t>rhema.vaithianathan@aut.ac.nz</t>
-  </si>
-  <si>
-    <t>Sandra</t>
-  </si>
-  <si>
-    <t>Velarde</t>
-  </si>
-  <si>
-    <t>sjvelarde@gmail.com</t>
-  </si>
-  <si>
-    <t>WSP</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>Villamor</t>
-  </si>
-  <si>
-    <t>Scion</t>
-  </si>
-  <si>
-    <t>Cameron</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
-    <t>cameron.walker@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Leilani</t>
-  </si>
-  <si>
-    <t>leilani.walker@aut.ac.nz</t>
-  </si>
-  <si>
-    <t>Krushil</t>
-  </si>
-  <si>
-    <t>Watene</t>
-  </si>
-  <si>
-    <t>krushil.watene@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Priscilla</t>
-  </si>
-  <si>
-    <t>Wehi</t>
-  </si>
-  <si>
-    <t>priscilla.wehi@otago.ac.nz</t>
-  </si>
-  <si>
-    <t>Hēmi</t>
-  </si>
-  <si>
-    <t>Whaanga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Massey University </t>
-  </si>
-  <si>
-    <t>Jesse</t>
-  </si>
-  <si>
-    <t>Whitehead</t>
-  </si>
-  <si>
-    <t>jesse.whitehead@waikato.ac.nz</t>
-  </si>
-  <si>
-    <t>University of Waikato/Nirai Research Ltd</t>
-  </si>
-  <si>
-    <t>Ōhaupō (Waikato)</t>
-  </si>
-  <si>
-    <t>Siouxsie</t>
-  </si>
-  <si>
-    <t>Wiles</t>
-  </si>
-  <si>
-    <t>s.wiles@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Phillip</t>
-  </si>
-  <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phillip.wilson@canterbury.ac.nz  </t>
-  </si>
-  <si>
-    <t>Ilze</t>
-  </si>
-  <si>
-    <t>Ziedins</t>
-  </si>
-  <si>
-    <t>i.ziedins@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Uli</t>
-  </si>
-  <si>
-    <t>Zuelicke</t>
-  </si>
-  <si>
-    <t>grace.villamor@scionresearch.com</t>
-  </si>
-  <si>
-    <t>i.c.castro@massey.ac.nz</t>
-  </si>
-  <si>
-    <t>lynn.riggs@productivity.govt.nz</t>
-  </si>
-  <si>
-    <t>william.godsoe@lincoln.ac.nz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">celine.cattoen-gilbert@niwa.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d.t.s.hayman@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">h.whaanga@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.liggins@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">matt.pinkerton@niwa.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">marcus.frean@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mubashir.qasim@dairynz.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">roudierp@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rebecca.priestley@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">binnyr@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uli.zuelicke@vuw.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">etheringtont@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">j.hunter1@massey.ac.nz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">macleodc@landcareresearch.co.nz </t>
-  </si>
-  <si>
-    <t>Christina</t>
-  </si>
-  <si>
-    <t>possibly also Alexandra</t>
-  </si>
-  <si>
-    <t>Cam</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Hamilton/ Gisborne</t>
-  </si>
-  <si>
-    <t>Jono</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Whangarei</t>
-  </si>
-  <si>
-    <t>Nicholas</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Phil</t>
-  </si>
-  <si>
-    <t>Cilla</t>
-  </si>
-  <si>
-    <t>Ulrich</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Thomas?</t>
-  </si>
-  <si>
-    <t>Other versions of their first name they use</t>
-  </si>
-  <si>
-    <t>Tabi</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>andrea.tabi@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Reju</t>
-  </si>
-  <si>
-    <t>reju.sam.john@auckland.ac.nz</t>
-  </si>
-  <si>
-    <t>Bernardo</t>
-  </si>
-  <si>
-    <t>Buarque</t>
-  </si>
-  <si>
-    <t>bbuarque@gmail.com</t>
-  </si>
-  <si>
-    <t>Kelley</t>
-  </si>
-  <si>
-    <t>dkel960@aucklanduni.ac.nz</t>
-  </si>
-  <si>
-    <t>Franca</t>
-  </si>
-  <si>
-    <t>Buelow</t>
-  </si>
-  <si>
-    <t>Virens</t>
-  </si>
-  <si>
-    <t>franca.buelow@canterbury.ac.nz</t>
-  </si>
-  <si>
-    <t>Beattie</t>
-  </si>
-  <si>
-    <t>alex.beattie@vuw.ac.nz</t>
-  </si>
-  <si>
-    <t>Victoria University of Wellington</t>
-  </si>
-  <si>
-    <t>Aisling</t>
-  </si>
-  <si>
-    <t>Rayne</t>
-  </si>
-  <si>
-    <t>aisling.rayne@cawthron.org.nz</t>
-  </si>
-  <si>
-    <t>evelynvirens@gmail.com</t>
-  </si>
-  <si>
-    <t>Evelyn</t>
-  </si>
-  <si>
-    <t>google_scholar_id</t>
-  </si>
-  <si>
-    <t>9zBBTb0AAAAJ</t>
-  </si>
-  <si>
-    <t>TSjPmycAAAAJ</t>
-  </si>
-  <si>
-    <t>8D8W8NsAAAAJ</t>
-  </si>
-  <si>
-    <t>scopus_au_id</t>
-  </si>
-  <si>
-    <t>Ic0ntsUAAAAJ</t>
-  </si>
-  <si>
-    <t>Xt1AACMAAAAJ</t>
-  </si>
-  <si>
-    <t>skip</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K9stBsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ymcd_j8AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>U075c-cAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>3svcBDsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1RfyVk4AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>q9BV9soAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HfQdgrcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>pqW61O0AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaderGYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>3SsqlCkAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0FInvU4AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>XCK_D0oAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>sE2Je-oAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VhX3VbwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>JhDH40UAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>mJlK_dwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PkUDCPsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZiUSYlMAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>g8DH5gYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>yINTHKsAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>jKnJDPMAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVEIwcQAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>pHjNU0gAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>hBdEqeYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mtn0TIwAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>80v_y-YAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>lqL9DsoAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>KuDLalcAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ze-7kTYAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>eLYlC84AAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>qRwdoDkAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>yi87D2cAAAAJ</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFsg92IAAAAJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1256,13 +1390,26 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1278,7 +1425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1295,6 +1442,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1311,10 +1464,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1617,7 +1766,7 @@
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1630,7 +1779,7 @@
     <col min="6" max="6" width="24.5" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1638,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1653,28 +1802,28 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>53</v>
@@ -1684,13 +1833,13 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I2">
         <v>56250119900</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1712,13 +1861,13 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I3">
         <v>55545943200</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1727,10 +1876,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -1739,16 +1888,16 @@
         <v>23</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I4">
         <v>7005704384</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1770,13 +1919,13 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I5">
         <v>18233378900</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1802,7 +1951,7 @@
         <v>57209398695</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1811,10 +1960,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
@@ -1824,13 +1973,13 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I7">
         <v>7005851367</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1839,10 +1988,10 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>236</v>
+        <v>384</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>49</v>
@@ -1851,21 +2000,26 @@
         <v>9</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="I8">
+        <v>14219508100</v>
+      </c>
       <c r="J8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
@@ -1874,9 +2028,14 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>333</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="I9">
+        <v>7402887425</v>
+      </c>
       <c r="J9">
         <v>1</v>
       </c>
@@ -1898,21 +2057,26 @@
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="I10">
+        <v>6603293321</v>
+      </c>
       <c r="J10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>160</v>
+        <v>387</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>41</v>
@@ -1920,7 +2084,12 @@
       <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="I11">
+        <v>8688520200</v>
+      </c>
       <c r="J11">
         <v>1</v>
       </c>
@@ -1934,7 +2103,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>62</v>
@@ -1942,21 +2111,26 @@
       <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="I12">
+        <v>9632564900</v>
+      </c>
       <c r="J12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>132</v>
@@ -1965,23 +2139,28 @@
         <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>195</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="I13">
+        <v>56030897200</v>
+      </c>
       <c r="J13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -1989,9 +2168,14 @@
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="I14">
+        <v>8590273100</v>
+      </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2012,11 +2196,16 @@
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>334</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="I15">
+        <v>16241337300</v>
+      </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2025,10 +2214,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>53</v>
@@ -2036,9 +2225,14 @@
       <c r="F16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="I16">
+        <v>8395488800</v>
+      </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2058,9 +2252,14 @@
       <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="I17">
+        <v>36668233300</v>
+      </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2081,8 +2280,11 @@
         <v>9</v>
       </c>
       <c r="H18" s="3"/>
+      <c r="I18">
+        <v>57287842200</v>
+      </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2094,7 +2296,7 @@
         <v>114</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -2103,23 +2305,28 @@
         <v>59</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="H19" s="4"/>
+        <v>335</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="I19">
+        <v>24376017100</v>
+      </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>22</v>
@@ -2127,21 +2334,26 @@
       <c r="F20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="I20">
+        <v>14322266400</v>
+      </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>18</v>
@@ -2149,9 +2361,14 @@
       <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="I21">
+        <v>57391641100</v>
+      </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2171,9 +2388,14 @@
       <c r="F22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="I22">
+        <v>23988357400</v>
+      </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2193,21 +2415,26 @@
       <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="I23">
+        <v>36704525400</v>
+      </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
@@ -2215,21 +2442,26 @@
       <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I24">
+        <v>56602470900</v>
+      </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>41</v>
@@ -2238,9 +2470,14 @@
         <v>9</v>
       </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I25">
+        <v>55114316000</v>
+      </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2261,9 +2498,14 @@
         <v>59</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="I26">
+        <v>7004092131</v>
+      </c>
       <c r="J26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2284,9 +2526,14 @@
         <v>28</v>
       </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="I27">
+        <v>7004267866</v>
+      </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2307,32 +2554,42 @@
         <v>42</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="I28">
+        <v>56928257900</v>
+      </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="I29">
+        <v>14629692200</v>
+      </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2353,9 +2610,14 @@
         <v>9</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="I30">
+        <v>8902993900</v>
+      </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2377,43 +2639,49 @@
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="3"/>
+      <c r="I31">
+        <v>58313215900</v>
+      </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="3"/>
+      <c r="I32">
+        <v>35365484000</v>
+      </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -2421,9 +2689,14 @@
       <c r="F33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I33">
+        <v>17339743000</v>
+      </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2444,44 +2717,54 @@
         <v>23</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="I34">
+        <v>57203528456</v>
+      </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="I35">
+        <v>12143371300</v>
+      </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>18</v>
@@ -2491,20 +2774,23 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="4"/>
+      <c r="I36">
+        <v>6603639295</v>
+      </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>22</v>
@@ -2514,43 +2800,51 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="4"/>
+      <c r="I37">
+        <v>25925460000</v>
+      </c>
       <c r="J37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="13" customFormat="1">
+      <c r="A38" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="4"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="I38" s="13">
+        <v>7102400791</v>
+      </c>
       <c r="J38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>53</v>
@@ -2560,30 +2854,38 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="3"/>
+      <c r="I39">
+        <v>14120027100</v>
+      </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="I40">
+        <v>57204169345</v>
+      </c>
       <c r="J40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2605,8 +2907,11 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="4"/>
+      <c r="I41">
+        <v>57270034900</v>
+      </c>
       <c r="J41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2618,7 +2923,7 @@
         <v>134</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
@@ -2627,21 +2932,26 @@
         <v>9</v>
       </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="I42">
+        <v>56461966900</v>
+      </c>
       <c r="J42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>53</v>
@@ -2650,34 +2960,44 @@
         <v>42</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="H43" s="4"/>
+        <v>337</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="I43">
+        <v>35575180300</v>
+      </c>
       <c r="J43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="8"/>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="I44">
+        <v>57201465027</v>
+      </c>
       <c r="J44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2699,8 +3019,11 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="3"/>
+      <c r="I45">
+        <v>57216492145</v>
+      </c>
       <c r="J45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2721,9 +3044,14 @@
         <v>9</v>
       </c>
       <c r="G46" s="8"/>
-      <c r="H46" s="3"/>
+      <c r="H46" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I46">
+        <v>36617114700</v>
+      </c>
       <c r="J46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2744,21 +3072,26 @@
         <v>9</v>
       </c>
       <c r="G47" s="8"/>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="I47">
+        <v>55877647600</v>
+      </c>
       <c r="J47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>49</v>
@@ -2768,8 +3101,11 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="4"/>
+      <c r="I48">
+        <v>55612294300</v>
+      </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2790,21 +3126,26 @@
         <v>28</v>
       </c>
       <c r="G49" s="8"/>
-      <c r="H49" s="3"/>
+      <c r="H49" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="I49">
+        <v>57193958261</v>
+      </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>141</v>
@@ -2813,9 +3154,14 @@
         <v>9</v>
       </c>
       <c r="G50" s="8"/>
-      <c r="H50" s="3"/>
+      <c r="H50" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I50">
+        <v>57190274432</v>
+      </c>
       <c r="J50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2827,7 +3173,7 @@
         <v>146</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>147</v>
@@ -2836,21 +3182,26 @@
         <v>9</v>
       </c>
       <c r="G51" s="8"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="I51">
+        <v>24474607700</v>
+      </c>
       <c r="J51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>49</v>
@@ -2859,32 +3210,40 @@
         <v>9</v>
       </c>
       <c r="G52" s="8"/>
-      <c r="H52" s="3"/>
+      <c r="H52" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="I52">
+        <v>55441246800</v>
+      </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="4"/>
+      <c r="I53">
+        <v>57225742769</v>
+      </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2912,14 +3271,14 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>18</v>
@@ -2942,7 +3301,7 @@
         <v>84</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>27</v>
@@ -3003,14 +3362,14 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>53</v>
@@ -3026,14 +3385,14 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>22</v>
@@ -3042,7 +3401,7 @@
         <v>23</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H60" s="4"/>
       <c r="J60">
@@ -3051,14 +3410,14 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>62</v>
@@ -3143,14 +3502,14 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>18</v>
@@ -3159,7 +3518,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H65" s="4"/>
       <c r="J65">
@@ -3168,14 +3527,14 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>53</v>
@@ -3184,7 +3543,7 @@
         <v>42</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H66" s="4"/>
       <c r="J66">
@@ -3193,17 +3552,17 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>14</v>
@@ -3229,7 +3588,7 @@
         <v>70</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G68" s="8"/>
       <c r="H68" s="4"/>
@@ -3239,7 +3598,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
@@ -3264,14 +3623,14 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>18</v>
@@ -3333,23 +3692,23 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H73" s="4"/>
       <c r="J73">
@@ -3358,14 +3717,14 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>53</v>
@@ -3374,7 +3733,7 @@
         <v>42</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H74" s="3"/>
       <c r="J74">
@@ -3383,14 +3742,14 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>41</v>
@@ -3406,14 +3765,14 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>22</v>
@@ -3422,7 +3781,7 @@
         <v>23</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H76" s="4"/>
       <c r="J76">
@@ -3431,14 +3790,14 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>49</v>
@@ -3507,7 +3866,7 @@
         <v>40</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>41</v>
@@ -3523,14 +3882,14 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>18</v>
@@ -3546,14 +3905,14 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>27</v>
@@ -3569,14 +3928,14 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>141</v>
@@ -3592,20 +3951,20 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G84" s="8"/>
       <c r="H84" s="4"/>
@@ -3638,20 +3997,20 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="F86" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G86" s="8"/>
       <c r="H86" s="4"/>
@@ -3661,14 +4020,14 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>49</v>
@@ -3707,14 +4066,14 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>128</v>
@@ -3730,14 +4089,14 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>18</v>
@@ -3776,14 +4135,14 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>27</v>
@@ -3799,14 +4158,14 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>53</v>
@@ -3822,20 +4181,20 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="4"/>
@@ -3875,7 +4234,7 @@
         <v>82</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>41</v>
@@ -3884,7 +4243,7 @@
         <v>42</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H96" s="4"/>
       <c r="J96">
@@ -3897,10 +4256,10 @@
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>132</v>
@@ -3941,14 +4300,14 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>27</v>
@@ -3957,7 +4316,7 @@
         <v>28</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H99" s="3"/>
       <c r="J99">
@@ -3973,7 +4332,7 @@
         <v>95</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>96</v>
@@ -3982,7 +4341,7 @@
         <v>42</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H100" s="4"/>
       <c r="J100">
@@ -3991,14 +4350,14 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>22</v>
@@ -4007,7 +4366,7 @@
         <v>23</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H101" s="3"/>
       <c r="J101">
@@ -4016,14 +4375,14 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>53</v>
@@ -4036,16 +4395,16 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B103" t="s">
+        <v>355</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>359</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>18</v>
@@ -4056,13 +4415,13 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>362</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>38</v>
@@ -4076,10 +4435,10 @@
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>18</v>
@@ -4090,16 +4449,16 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J106">
         <v>1</v>
@@ -4107,13 +4466,13 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D107" s="4" t="s">
         <v>366</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>53</v>
@@ -4127,13 +4486,13 @@
         <v>135</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -4141,13 +4500,13 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>372</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>128</v>
@@ -4160,6 +4519,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F102">
     <sortCondition ref="A2:A102"/>
   </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
added gpt author prediction, google scholar and scopus abstarct retrival
</commit_message>
<xml_diff>
--- a/TPM 2023 Principal Investigators.xlsx
+++ b/TPM 2023 Principal Investigators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzhu986\PycharmProjects\Pub_Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A7CA94-E630-4AA2-93DC-41098718EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37A462A-0710-46DF-9823-A83D5C78AB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{42F0867C-C5B5-7247-966A-65285227E76E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="477">
   <si>
     <t>First Name</t>
   </si>
@@ -1051,9 +1051,6 @@
   </si>
   <si>
     <t>Nicholas</t>
-  </si>
-  <si>
-    <t>Peter</t>
   </si>
   <si>
     <t>Phil</t>
@@ -1325,13 +1322,197 @@
   </si>
   <si>
     <t>EFsg92IAAAAJ</t>
+  </si>
+  <si>
+    <t>hLaHjh8AAAAJ</t>
+  </si>
+  <si>
+    <t>80aVSRcAAAAJ</t>
+  </si>
+  <si>
+    <t>fu9lhjoAAAAJ</t>
+  </si>
+  <si>
+    <t>zEqatoMAAAAJ</t>
+  </si>
+  <si>
+    <t>H2ONJ40AAAAJ</t>
+  </si>
+  <si>
+    <t>AZT37l0AAAAJ</t>
+  </si>
+  <si>
+    <t>RZY0o9sAAAAJ</t>
+  </si>
+  <si>
+    <t>ZUXmQvoAAAAJ</t>
+  </si>
+  <si>
+    <t>https://profiles.waikato.ac.nz/maui.hudson/publications</t>
+  </si>
+  <si>
+    <t>https://www.cawthron.org.nz/our-people/mckayla-holloway/</t>
+  </si>
+  <si>
+    <t>sTqXyfwAAAAJ</t>
+  </si>
+  <si>
+    <t>Q5MZLZQAAAAJ</t>
+  </si>
+  <si>
+    <t>multpul uni result on google scholar</t>
+  </si>
+  <si>
+    <t>3Cg41TgAAAAJ</t>
+  </si>
+  <si>
+    <t>o21NL1YAAAAJ</t>
+  </si>
+  <si>
+    <t>r80SLXsAAAAJ</t>
+  </si>
+  <si>
+    <t>KRO8OiYAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Pauline-Harris</t>
+  </si>
+  <si>
+    <t>IT1NN5oAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.otago.ac.nz/marinescience/people/staff/dr-pete-russell</t>
+  </si>
+  <si>
+    <r>
+      <t>Pete</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="double"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <t>8mj45JQAAAAJ</t>
+  </si>
+  <si>
+    <t>e0eWjnwAAAAJ</t>
+  </si>
+  <si>
+    <t>ROBMhaUAAAAJ</t>
+  </si>
+  <si>
+    <t>OGOFzGMAAAAJ</t>
+  </si>
+  <si>
+    <t>wEqs8pkAAAAJ</t>
+  </si>
+  <si>
+    <t>tU-6CiYAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.teipukarea.maori.nz/the-team/dr-rachael-kaai-mahuta</t>
+  </si>
+  <si>
+    <t>nudTp0UAAAAJ</t>
+  </si>
+  <si>
+    <t>sdQGx1QAAAAJ</t>
+  </si>
+  <si>
+    <t>biprEiMAAAAJ</t>
+  </si>
+  <si>
+    <t>jpD_uAwAAAAJ</t>
+  </si>
+  <si>
+    <t>ZOSKcOcAAAAJ</t>
+  </si>
+  <si>
+    <t>mSBxGo4AAAAJ</t>
+  </si>
+  <si>
+    <t>g8DvOJgAAAAJ</t>
+  </si>
+  <si>
+    <t>GujKmrQAAAAJ</t>
+  </si>
+  <si>
+    <t>RHyTIvMAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.cawthron.org.nz/our-people/simon-stewart/
+https://www.researchgate.net/profile/Simon-Stewart-3</t>
+  </si>
+  <si>
+    <t>i4UolSMAAAAJ</t>
+  </si>
+  <si>
+    <t>ZCtn3kYAAAAJ</t>
+  </si>
+  <si>
+    <t>BhII4jEAAAAJ</t>
+  </si>
+  <si>
+    <t>XfFhVhAAAAAJ</t>
+  </si>
+  <si>
+    <t>dC17nbIAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.biosecurity-toolbox.org.nz/staff-member/te-rerekohu-tuterangiwhiu/</t>
+  </si>
+  <si>
+    <t>d3OQ51IAAAAJ</t>
+  </si>
+  <si>
+    <t>7FJfUN8AAAAJ</t>
+  </si>
+  <si>
+    <t>XgKumXgAAAAJ</t>
+  </si>
+  <si>
+    <t>jjUHqkYAAAAJ</t>
+  </si>
+  <si>
+    <t>ttOVsTQAAAAJ</t>
+  </si>
+  <si>
+    <t>https://www.otago.ac.nz/archaeology/people/zac-mcivor</t>
+  </si>
+  <si>
+    <t>hvFqEvIAAAAJ</t>
+  </si>
+  <si>
+    <t>EeZSlzsAAAAJ</t>
+  </si>
+  <si>
+    <t>https://profiles.auckland.ac.nz/david-kelley/publications</t>
+  </si>
+  <si>
+    <t>GOTCXqEAAAAJ</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-2328-5024</t>
+  </si>
+  <si>
+    <t>AgcLciMAAAAJ</t>
+  </si>
+  <si>
+    <t>gm7qbskAAAAJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1397,8 +1578,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u val="double"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1408,6 +1596,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1425,7 +1619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1448,6 +1642,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1763,10 +1961,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8B157A-D10D-D949-B41A-E7AC1C9C79E8}">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1780,6 +1979,7 @@
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1787,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1802,16 +2002,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1833,13 +2033,13 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I2">
         <v>56250119900</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1861,13 +2061,13 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I3">
         <v>55545943200</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1891,13 +2091,13 @@
         <v>332</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I4">
         <v>7005704384</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1919,13 +2119,13 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I5">
         <v>18233378900</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1951,7 +2151,7 @@
         <v>57209398695</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1973,13 +2173,13 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I7">
         <v>7005851367</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1988,7 +2188,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>235</v>
@@ -2001,13 +2201,13 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I8">
         <v>14219508100</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2031,13 +2231,13 @@
         <v>333</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I9">
         <v>7402887425</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2058,18 +2258,18 @@
         <v>9</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I10">
         <v>6603293321</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -2085,13 +2285,13 @@
         <v>23</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I11">
         <v>8688520200</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2112,13 +2312,13 @@
         <v>42</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I12">
         <v>9632564900</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2142,13 +2342,13 @@
         <v>195</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I13">
         <v>56030897200</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2169,7 +2369,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I14">
         <v>8590273100</v>
@@ -2199,7 +2399,7 @@
         <v>334</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I15">
         <v>16241337300</v>
@@ -2226,7 +2426,7 @@
         <v>42</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I16">
         <v>8395488800</v>
@@ -2253,7 +2453,7 @@
         <v>9</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I17">
         <v>36668233300</v>
@@ -2308,7 +2508,7 @@
         <v>335</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I19">
         <v>24376017100</v>
@@ -2335,7 +2535,7 @@
         <v>28</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I20">
         <v>14322266400</v>
@@ -2362,7 +2562,7 @@
         <v>9</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I21">
         <v>57391641100</v>
@@ -2389,7 +2589,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I22">
         <v>23988357400</v>
@@ -2416,7 +2616,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I23">
         <v>36704525400</v>
@@ -2443,7 +2643,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I24">
         <v>56602470900</v>
@@ -2471,7 +2671,7 @@
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I25">
         <v>55114316000</v>
@@ -2499,7 +2699,7 @@
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I26">
         <v>7004092131</v>
@@ -2527,7 +2727,7 @@
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I27">
         <v>7004267866</v>
@@ -2555,7 +2755,7 @@
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I28">
         <v>56928257900</v>
@@ -2583,7 +2783,7 @@
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I29">
         <v>14629692200</v>
@@ -2611,7 +2811,7 @@
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I30">
         <v>8902993900</v>
@@ -2690,7 +2890,7 @@
         <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I33">
         <v>17339743000</v>
@@ -2718,7 +2918,7 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I34">
         <v>57203528456</v>
@@ -2746,7 +2946,7 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I35">
         <v>12143371300</v>
@@ -2826,7 +3026,7 @@
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I38" s="13">
         <v>7102400791</v>
@@ -2879,7 +3079,7 @@
         <v>301</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I40">
         <v>57204169345</v>
@@ -2933,7 +3133,7 @@
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I42">
         <v>56461966900</v>
@@ -2963,7 +3163,7 @@
         <v>337</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I43">
         <v>35575180300</v>
@@ -2991,7 +3191,7 @@
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I44">
         <v>57201465027</v>
@@ -3045,7 +3245,7 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I46">
         <v>36617114700</v>
@@ -3073,7 +3273,7 @@
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I47">
         <v>55877647600</v>
@@ -3108,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:11">
       <c r="A49" s="2" t="s">
         <v>119</v>
       </c>
@@ -3127,7 +3327,7 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I49">
         <v>57193958261</v>
@@ -3136,7 +3336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:11">
       <c r="A50" s="2" t="s">
         <v>286</v>
       </c>
@@ -3155,7 +3355,7 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I50">
         <v>57190274432</v>
@@ -3164,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:11">
       <c r="A51" s="2" t="s">
         <v>145</v>
       </c>
@@ -3183,7 +3383,7 @@
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I51">
         <v>24474607700</v>
@@ -3192,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:11">
       <c r="A52" s="2" t="s">
         <v>204</v>
       </c>
@@ -3211,7 +3411,7 @@
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I52">
         <v>55441246800</v>
@@ -3220,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:11">
       <c r="A53" s="2" t="s">
         <v>220</v>
       </c>
@@ -3246,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:11">
       <c r="A54" s="2" t="s">
         <v>74</v>
       </c>
@@ -3264,12 +3464,17 @@
         <v>28</v>
       </c>
       <c r="G54" s="8"/>
-      <c r="H54" s="4"/>
+      <c r="H54" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="I54">
+        <v>35322074400</v>
+      </c>
       <c r="J54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="2" t="s">
         <v>180</v>
       </c>
@@ -3287,12 +3492,17 @@
         <v>9</v>
       </c>
       <c r="G55" s="8"/>
-      <c r="H55" s="4"/>
+      <c r="H55" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="I55">
+        <v>40762034000</v>
+      </c>
       <c r="J55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="2" t="s">
         <v>83</v>
       </c>
@@ -3309,12 +3519,17 @@
       <c r="F56" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="I56">
+        <v>8358660400</v>
+      </c>
       <c r="J56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="2" t="s">
         <v>88</v>
       </c>
@@ -3332,12 +3547,17 @@
         <v>9</v>
       </c>
       <c r="G57" s="8"/>
-      <c r="H57" s="3"/>
+      <c r="H57" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="I57">
+        <v>55970397200</v>
+      </c>
       <c r="J57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="2" t="s">
         <v>154</v>
       </c>
@@ -3355,12 +3575,17 @@
         <v>28</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="H58" s="4"/>
+      <c r="H58" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="I58">
+        <v>57210110677</v>
+      </c>
       <c r="J58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="2" t="s">
         <v>213</v>
       </c>
@@ -3378,12 +3603,17 @@
         <v>42</v>
       </c>
       <c r="G59" s="8"/>
-      <c r="H59" s="4"/>
+      <c r="H59" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="I59">
+        <v>36752990300</v>
+      </c>
       <c r="J59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="2" t="s">
         <v>338</v>
       </c>
@@ -3403,12 +3633,20 @@
       <c r="G60" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="H60" s="4"/>
+      <c r="H60" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="I60">
+        <v>8361414000</v>
+      </c>
       <c r="J60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K60" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="2" t="s">
         <v>198</v>
       </c>
@@ -3426,12 +3664,17 @@
         <v>28</v>
       </c>
       <c r="G61" s="8"/>
-      <c r="H61" s="3"/>
+      <c r="H61" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="I61">
+        <v>7003793212</v>
+      </c>
       <c r="J61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
         <v>129</v>
       </c>
@@ -3450,11 +3693,17 @@
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="4"/>
+      <c r="I62">
+        <v>16678829800</v>
+      </c>
       <c r="J62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -3474,10 +3723,13 @@
       <c r="G63" s="8"/>
       <c r="H63" s="3"/>
       <c r="J63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
@@ -3495,12 +3747,17 @@
         <v>9</v>
       </c>
       <c r="G64" s="8"/>
-      <c r="H64" s="4"/>
+      <c r="H64" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="I64">
+        <v>7404105542</v>
+      </c>
       <c r="J64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="2" t="s">
         <v>192</v>
       </c>
@@ -3520,12 +3777,20 @@
       <c r="G65" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="H65" s="4"/>
+      <c r="H65" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="I65">
+        <v>57209018448</v>
+      </c>
       <c r="J65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K65" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="2" t="s">
         <v>192</v>
       </c>
@@ -3545,12 +3810,20 @@
       <c r="G66" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="H66" s="4"/>
+      <c r="H66" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="I66">
+        <v>6603773075</v>
+      </c>
       <c r="J66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K66" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="5" t="s">
         <v>217</v>
       </c>
@@ -3568,12 +3841,17 @@
         <v>14</v>
       </c>
       <c r="G67" s="8"/>
-      <c r="H67" s="4"/>
+      <c r="H67" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="I67">
+        <v>57191504787</v>
+      </c>
       <c r="J67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
@@ -3591,12 +3869,17 @@
         <v>340</v>
       </c>
       <c r="G68" s="8"/>
-      <c r="H68" s="4"/>
+      <c r="H68" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="I68">
+        <v>8699959500</v>
+      </c>
       <c r="J68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="2" t="s">
         <v>341</v>
       </c>
@@ -3616,12 +3899,17 @@
       <c r="G69" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="I69">
+        <v>8598859700</v>
+      </c>
       <c r="J69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="2" t="s">
         <v>186</v>
       </c>
@@ -3640,11 +3928,14 @@
       </c>
       <c r="G70" s="8"/>
       <c r="H70" s="4"/>
+      <c r="I70">
+        <v>7102069328</v>
+      </c>
       <c r="J70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="2" t="s">
         <v>106</v>
       </c>
@@ -3663,11 +3954,17 @@
       </c>
       <c r="G71" s="8"/>
       <c r="H71" s="4"/>
+      <c r="I71">
+        <v>57199072952</v>
+      </c>
       <c r="J71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="2" t="s">
         <v>85</v>
       </c>
@@ -3685,14 +3982,19 @@
         <v>42</v>
       </c>
       <c r="G72" s="8"/>
-      <c r="H72" s="3"/>
+      <c r="H72" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="I72">
+        <v>57200755784</v>
+      </c>
       <c r="J72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="6" t="s">
-        <v>342</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="14" t="s">
+        <v>440</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
@@ -3710,12 +4012,20 @@
       <c r="G73" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="H73" s="4"/>
+      <c r="H73" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="I73">
+        <v>55603241700</v>
+      </c>
       <c r="J73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="2" t="s">
         <v>305</v>
       </c>
@@ -3733,14 +4043,19 @@
         <v>42</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="H74" s="3"/>
+        <v>342</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="I74">
+        <v>8410912000</v>
+      </c>
       <c r="J74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="2" t="s">
         <v>225</v>
       </c>
@@ -3758,12 +4073,17 @@
         <v>59</v>
       </c>
       <c r="G75" s="8"/>
-      <c r="H75" s="4"/>
+      <c r="H75" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I75">
+        <v>24391496200</v>
+      </c>
       <c r="J75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="2" t="s">
         <v>291</v>
       </c>
@@ -3781,14 +4101,19 @@
         <v>23</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="H76" s="4"/>
+        <v>343</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I76">
+        <v>14014354900</v>
+      </c>
       <c r="J76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="2" t="s">
         <v>253</v>
       </c>
@@ -3806,12 +4131,17 @@
         <v>9</v>
       </c>
       <c r="G77" s="8"/>
-      <c r="H77" s="4"/>
+      <c r="H77" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="I77">
+        <v>35786615800</v>
+      </c>
       <c r="J77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="2" t="s">
         <v>29</v>
       </c>
@@ -3829,12 +4159,17 @@
         <v>9</v>
       </c>
       <c r="G78" s="8"/>
-      <c r="H78" s="3"/>
+      <c r="H78" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I78">
+        <v>22633898400</v>
+      </c>
       <c r="J78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="2" t="s">
         <v>138</v>
       </c>
@@ -3853,11 +4188,17 @@
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="4"/>
+      <c r="I79">
+        <v>57213193223</v>
+      </c>
       <c r="J79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="2" t="s">
         <v>39</v>
       </c>
@@ -3875,12 +4216,17 @@
         <v>42</v>
       </c>
       <c r="G80" s="8"/>
-      <c r="H80" s="4"/>
+      <c r="H80" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="I80">
+        <v>56648035300</v>
+      </c>
       <c r="J80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="2" t="s">
         <v>201</v>
       </c>
@@ -3898,12 +4244,17 @@
         <v>9</v>
       </c>
       <c r="G81" s="8"/>
-      <c r="H81" s="4"/>
+      <c r="H81" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="I81">
+        <v>36089317600</v>
+      </c>
       <c r="J81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="2" t="s">
         <v>201</v>
       </c>
@@ -3921,12 +4272,17 @@
         <v>28</v>
       </c>
       <c r="G82" s="8"/>
-      <c r="H82" s="4"/>
+      <c r="H82" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="I82">
+        <v>14051120200</v>
+      </c>
       <c r="J82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="2" t="s">
         <v>273</v>
       </c>
@@ -3944,12 +4300,17 @@
         <v>9</v>
       </c>
       <c r="G83" s="8"/>
-      <c r="H83" s="3"/>
+      <c r="H83" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="I83">
+        <v>6602352226</v>
+      </c>
       <c r="J83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="2" t="s">
         <v>231</v>
       </c>
@@ -3967,12 +4328,17 @@
         <v>234</v>
       </c>
       <c r="G84" s="8"/>
-      <c r="H84" s="4"/>
+      <c r="H84" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="I84">
+        <v>56246037800</v>
+      </c>
       <c r="J84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -3990,12 +4356,17 @@
         <v>28</v>
       </c>
       <c r="G85" s="8"/>
-      <c r="H85" s="4"/>
+      <c r="H85" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="I85">
+        <v>15070007200</v>
+      </c>
       <c r="J85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="2" t="s">
         <v>276</v>
       </c>
@@ -4013,12 +4384,17 @@
         <v>272</v>
       </c>
       <c r="G86" s="8"/>
-      <c r="H86" s="4"/>
+      <c r="H86" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="I86">
+        <v>16040823900</v>
+      </c>
       <c r="J86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="2" t="s">
         <v>183</v>
       </c>
@@ -4036,12 +4412,17 @@
         <v>9</v>
       </c>
       <c r="G87" s="8"/>
-      <c r="H87" s="4"/>
+      <c r="H87" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="I87">
+        <v>57204946580</v>
+      </c>
       <c r="J87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="2" t="s">
         <v>115</v>
       </c>
@@ -4059,12 +4440,17 @@
         <v>118</v>
       </c>
       <c r="G88" s="8"/>
-      <c r="H88" s="3"/>
+      <c r="H88" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="I88">
+        <v>6603876052</v>
+      </c>
       <c r="J88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="31.5">
       <c r="A89" s="2" t="s">
         <v>248</v>
       </c>
@@ -4082,12 +4468,20 @@
         <v>118</v>
       </c>
       <c r="G89" s="8"/>
-      <c r="H89" s="4"/>
+      <c r="H89" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="I89">
+        <v>7401747189</v>
+      </c>
       <c r="J89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K89" s="15" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="2" t="s">
         <v>302</v>
       </c>
@@ -4105,12 +4499,17 @@
         <v>9</v>
       </c>
       <c r="G90" s="8"/>
-      <c r="H90" s="3"/>
+      <c r="H90" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="I90">
+        <v>6603848952</v>
+      </c>
       <c r="J90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="2" t="s">
         <v>148</v>
       </c>
@@ -4128,12 +4527,17 @@
         <v>9</v>
       </c>
       <c r="G91" s="8"/>
-      <c r="H91" s="3"/>
+      <c r="H91" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="I91">
+        <v>16233735500</v>
+      </c>
       <c r="J91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="2" t="s">
         <v>163</v>
       </c>
@@ -4151,12 +4555,17 @@
         <v>28</v>
       </c>
       <c r="G92" s="8"/>
-      <c r="H92" s="3"/>
+      <c r="H92" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="I92">
+        <v>7004258982</v>
+      </c>
       <c r="J92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="2" t="s">
         <v>245</v>
       </c>
@@ -4174,12 +4583,17 @@
         <v>42</v>
       </c>
       <c r="G93" s="8"/>
-      <c r="H93" s="4"/>
+      <c r="H93" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="I93">
+        <v>7004361366</v>
+      </c>
       <c r="J93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="2" t="s">
         <v>269</v>
       </c>
@@ -4198,11 +4612,17 @@
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="4"/>
+      <c r="I94">
+        <v>58139745200</v>
+      </c>
       <c r="J94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="2" t="s">
         <v>142</v>
       </c>
@@ -4220,12 +4640,17 @@
         <v>9</v>
       </c>
       <c r="G95" s="8"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="I95">
+        <v>6602231449</v>
+      </c>
       <c r="J95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="2" t="s">
         <v>81</v>
       </c>
@@ -4243,14 +4668,19 @@
         <v>42</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H96" s="4"/>
+        <v>347</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="I96">
+        <v>22333495600</v>
+      </c>
       <c r="J96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="2" t="s">
         <v>81</v>
       </c>
@@ -4269,11 +4699,14 @@
       </c>
       <c r="G97" s="8"/>
       <c r="H97" s="4"/>
+      <c r="I97">
+        <v>35364908100</v>
+      </c>
       <c r="J97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="2" t="s">
         <v>35</v>
       </c>
@@ -4293,12 +4726,17 @@
       <c r="G98" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H98" s="4"/>
+      <c r="H98" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="I98">
+        <v>56730622300</v>
+      </c>
       <c r="J98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="2" t="s">
         <v>311</v>
       </c>
@@ -4316,14 +4754,19 @@
         <v>28</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="H99" s="3"/>
+        <v>344</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="I99">
+        <v>55971424300</v>
+      </c>
       <c r="J99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="2" t="s">
         <v>94</v>
       </c>
@@ -4341,14 +4784,19 @@
         <v>42</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="H100" s="4"/>
+        <v>345</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="I100">
+        <v>24281036500</v>
+      </c>
       <c r="J100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="2" t="s">
         <v>171</v>
       </c>
@@ -4366,153 +4814,203 @@
         <v>23</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="H101" s="3"/>
+        <v>346</v>
+      </c>
+      <c r="H101" s="4"/>
+      <c r="I101">
+        <v>56971215000</v>
+      </c>
       <c r="J101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K101" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
+      <c r="H102" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="I102">
+        <v>50263224000</v>
+      </c>
       <c r="J102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B103" t="s">
+        <v>354</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="B103" t="s">
-        <v>355</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H103" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="I103">
+        <v>57206562038</v>
+      </c>
       <c r="J103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="H104" s="4"/>
+      <c r="I104">
+        <v>57205731410</v>
+      </c>
       <c r="J104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>361</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>362</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H105" s="4"/>
       <c r="J105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="K105" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="H106" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="I106">
+        <v>57202438912</v>
+      </c>
       <c r="J106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="D107" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="H107" s="4"/>
+      <c r="I107">
+        <v>57201559210</v>
+      </c>
       <c r="J107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K107" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="E108" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="H108" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="I108">
+        <v>57218876434</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="J108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="D109" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="H109" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="I109">
+        <v>57214152104</v>
+      </c>
       <c r="J109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4611,8 +5109,18 @@
     <hyperlink ref="D108" r:id="rId76" xr:uid="{63F14034-90CD-49FC-B022-7FFEC8F52224}"/>
     <hyperlink ref="D109" r:id="rId77" xr:uid="{6536C4C8-6498-4E12-B6B1-B97FF48DDF4A}"/>
     <hyperlink ref="D106" r:id="rId78" xr:uid="{40BD8D95-5BB3-48F3-8573-BD80342BEE12}"/>
+    <hyperlink ref="K62" r:id="rId79" xr:uid="{EFD15F24-4C69-4399-8FBE-C43788AD740C}"/>
+    <hyperlink ref="K63" r:id="rId80" xr:uid="{785056D3-2A9B-451F-96D3-C1762A801AFD}"/>
+    <hyperlink ref="K71" r:id="rId81" xr:uid="{EFFD08D8-009D-4A9F-B96F-97AE66F1846A}"/>
+    <hyperlink ref="K73" r:id="rId82" xr:uid="{8730D6A2-F593-4735-9450-8F38C1D3F353}"/>
+    <hyperlink ref="K79" r:id="rId83" xr:uid="{7EF6A628-D375-4827-9C50-8B739CF71C13}"/>
+    <hyperlink ref="K89" r:id="rId84" display="https://www.cawthron.org.nz/our-people/simon-stewart/" xr:uid="{FBDA06A5-62E7-4A94-B61C-CC4D6F5748BD}"/>
+    <hyperlink ref="K94" r:id="rId85" xr:uid="{C5AAC686-F004-4566-8494-0BB1D384FF0B}"/>
+    <hyperlink ref="K101" r:id="rId86" xr:uid="{E7A676A2-9052-4016-991A-65475BEB272A}"/>
+    <hyperlink ref="K105" r:id="rId87" xr:uid="{2D17FEC9-3ADC-440A-B7A3-80597CF5D6DC}"/>
+    <hyperlink ref="K107" r:id="rId88" xr:uid="{40FEF1DE-56BE-4465-974B-EE943146D224}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId89"/>
 </worksheet>
 </file>
</xml_diff>